<commit_message>
Finished classes description Minor refactorings
</commit_message>
<xml_diff>
--- a/Documentation/Class descriptions.xlsx
+++ b/Documentation/Class descriptions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pauldanilin/Documents/HSE/CourseWorks/HistogramModel/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46564E13-D997-F340-9DE6-8DAC77A9266F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CD3D197-BF38-D54A-A9C8-1944831F20AD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{0CA7BCAD-690E-1A42-B7BF-CE8354672EFF}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="841" uniqueCount="200">
   <si>
     <t>Класс</t>
   </si>
@@ -454,6 +454,177 @@
   </si>
   <si>
     <t>Преобразует узел дерева</t>
+  </si>
+  <si>
+    <t>BinaryOperationNode</t>
+  </si>
+  <si>
+    <t>operation</t>
+  </si>
+  <si>
+    <t>left</t>
+  </si>
+  <si>
+    <t>right</t>
+  </si>
+  <si>
+    <t>UnaryOperationNode</t>
+  </si>
+  <si>
+    <t>Операция в узле</t>
+  </si>
+  <si>
+    <t>Левое поддерево</t>
+  </si>
+  <si>
+    <t>Правое поддерево</t>
+  </si>
+  <si>
+    <t>Поддерево</t>
+  </si>
+  <si>
+    <t>AggregateOperationNode</t>
+  </si>
+  <si>
+    <t>AggregateOperation</t>
+  </si>
+  <si>
+    <t>Гистограмма в узле</t>
+  </si>
+  <si>
+    <t>SubhistogramNode</t>
+  </si>
+  <si>
+    <t>properties</t>
+  </si>
+  <si>
+    <t>originOpt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Option[Node[E]] </t>
+  </si>
+  <si>
+    <t>Подмножество</t>
+  </si>
+  <si>
+    <t>Поддерево узла</t>
+  </si>
+  <si>
+    <t>OperationInput</t>
+  </si>
+  <si>
+    <t>Вводимая операция</t>
+  </si>
+  <si>
+    <t>SubhistogramInput</t>
+  </si>
+  <si>
+    <t>Подмножество элементов</t>
+  </si>
+  <si>
+    <t>HistogramInput</t>
+  </si>
+  <si>
+    <t>Гистограмма</t>
+  </si>
+  <si>
+    <t>Parser</t>
+  </si>
+  <si>
+    <t>parse</t>
+  </si>
+  <si>
+    <t>Option[Stack[Input[E]]]</t>
+  </si>
+  <si>
+    <t>query: String, implicit aliasToInput: Map[String, Input[E]]</t>
+  </si>
+  <si>
+    <t>getLexems</t>
+  </si>
+  <si>
+    <t>query: String, acc: Stack[Input[E]], aliasToInput: Map[String, Input[E]]</t>
+  </si>
+  <si>
+    <t>toPolishNotation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stack[Input[E]] </t>
+  </si>
+  <si>
+    <t>query: Stack[Input[E]], resultAcc: Stack[Input[E]], operandsAcc: Stack[Input[E]]</t>
+  </si>
+  <si>
+    <t>Преобразует последовательность входов в польскую инверсную последовательность</t>
+  </si>
+  <si>
+    <t>Преобразует строку в последовательность входных конструкций</t>
+  </si>
+  <si>
+    <t>Преобразует строку в последовательность входных лексем в польской нотации</t>
+  </si>
+  <si>
+    <t>TreeExecutor</t>
+  </si>
+  <si>
+    <t>execute</t>
+  </si>
+  <si>
+    <t>Either[Histogram[E], Double]</t>
+  </si>
+  <si>
+    <t>tree: Node[E]</t>
+  </si>
+  <si>
+    <t>Исполняет вычисления на АСТ</t>
+  </si>
+  <si>
+    <t>Query</t>
+  </si>
+  <si>
+    <t>root</t>
+  </si>
+  <si>
+    <t>АСТ</t>
+  </si>
+  <si>
+    <t>parseStack</t>
+  </si>
+  <si>
+    <t>fromString</t>
+  </si>
+  <si>
+    <t>standardAliases</t>
+  </si>
+  <si>
+    <t>Map[String, Input[E]]</t>
+  </si>
+  <si>
+    <t>Стандартные алиасы входных конструкций</t>
+  </si>
+  <si>
+    <t>Исполняет запрос</t>
+  </si>
+  <si>
+    <t>Преобразует польскую запись в АСТ входных конструкций</t>
+  </si>
+  <si>
+    <t>operationsStack: Stack[Input[E]]</t>
+  </si>
+  <si>
+    <t>Query[E]</t>
+  </si>
+  <si>
+    <t>Stack[Input[E]]</t>
+  </si>
+  <si>
+    <t>Формирует запрос по последовательности входных конструкций</t>
+  </si>
+  <si>
+    <t>query: String, aliasToInput: Map[String, Input[E]]</t>
+  </si>
+  <si>
+    <t>Формирует запрос по строковому представлению</t>
   </si>
 </sst>
 </file>
@@ -497,9 +668,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -814,10 +988,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E908023-0F4A-F746-8F0C-8318E7AD5793}">
-  <dimension ref="A1:E211"/>
+  <dimension ref="A1:E296"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A197" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D214" sqref="D214"/>
+    <sheetView tabSelected="1" topLeftCell="A275" zoomScale="150" workbookViewId="0">
+      <selection activeCell="E297" sqref="E297"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2973,6 +3147,889 @@
         <v>142</v>
       </c>
     </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A213" t="s">
+        <v>0</v>
+      </c>
+      <c r="B213" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A214" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A215" t="s">
+        <v>2</v>
+      </c>
+      <c r="B215" t="s">
+        <v>5</v>
+      </c>
+      <c r="C215" t="s">
+        <v>3</v>
+      </c>
+      <c r="D215" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A216" t="s">
+        <v>144</v>
+      </c>
+      <c r="B216" t="s">
+        <v>10</v>
+      </c>
+      <c r="C216" t="s">
+        <v>101</v>
+      </c>
+      <c r="D216" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A217" t="s">
+        <v>145</v>
+      </c>
+      <c r="B217" t="s">
+        <v>10</v>
+      </c>
+      <c r="C217" t="s">
+        <v>141</v>
+      </c>
+      <c r="D217" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A218" t="s">
+        <v>146</v>
+      </c>
+      <c r="B218" t="s">
+        <v>10</v>
+      </c>
+      <c r="C218" t="s">
+        <v>141</v>
+      </c>
+      <c r="D218" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A219" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A220" t="s">
+        <v>2</v>
+      </c>
+      <c r="B220" t="s">
+        <v>5</v>
+      </c>
+      <c r="C220" t="s">
+        <v>3</v>
+      </c>
+      <c r="D220" t="s">
+        <v>7</v>
+      </c>
+      <c r="E220" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A221" t="s">
+        <v>139</v>
+      </c>
+      <c r="B221" t="s">
+        <v>10</v>
+      </c>
+      <c r="C221" t="s">
+        <v>141</v>
+      </c>
+      <c r="D221" t="s">
+        <v>140</v>
+      </c>
+      <c r="E221" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A223" t="s">
+        <v>0</v>
+      </c>
+      <c r="B223" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A224" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A225" t="s">
+        <v>2</v>
+      </c>
+      <c r="B225" t="s">
+        <v>5</v>
+      </c>
+      <c r="C225" t="s">
+        <v>3</v>
+      </c>
+      <c r="D225" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A226" t="s">
+        <v>144</v>
+      </c>
+      <c r="B226" t="s">
+        <v>10</v>
+      </c>
+      <c r="C226" t="s">
+        <v>99</v>
+      </c>
+      <c r="D226" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A227" t="s">
+        <v>87</v>
+      </c>
+      <c r="B227" t="s">
+        <v>10</v>
+      </c>
+      <c r="C227" t="s">
+        <v>141</v>
+      </c>
+      <c r="D227" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A228" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A229" t="s">
+        <v>2</v>
+      </c>
+      <c r="B229" t="s">
+        <v>5</v>
+      </c>
+      <c r="C229" t="s">
+        <v>3</v>
+      </c>
+      <c r="D229" t="s">
+        <v>7</v>
+      </c>
+      <c r="E229" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A230" t="s">
+        <v>139</v>
+      </c>
+      <c r="B230" t="s">
+        <v>10</v>
+      </c>
+      <c r="C230" t="s">
+        <v>141</v>
+      </c>
+      <c r="D230" t="s">
+        <v>140</v>
+      </c>
+      <c r="E230" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A232" t="s">
+        <v>0</v>
+      </c>
+      <c r="B232" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A233" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A234" t="s">
+        <v>2</v>
+      </c>
+      <c r="B234" t="s">
+        <v>5</v>
+      </c>
+      <c r="C234" t="s">
+        <v>3</v>
+      </c>
+      <c r="D234" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A235" t="s">
+        <v>144</v>
+      </c>
+      <c r="B235" t="s">
+        <v>10</v>
+      </c>
+      <c r="C235" t="s">
+        <v>153</v>
+      </c>
+      <c r="D235" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A236" t="s">
+        <v>145</v>
+      </c>
+      <c r="B236" t="s">
+        <v>10</v>
+      </c>
+      <c r="C236" t="s">
+        <v>141</v>
+      </c>
+      <c r="D236" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A237" t="s">
+        <v>146</v>
+      </c>
+      <c r="B237" t="s">
+        <v>10</v>
+      </c>
+      <c r="C237" t="s">
+        <v>141</v>
+      </c>
+      <c r="D237" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A238" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A239" t="s">
+        <v>2</v>
+      </c>
+      <c r="B239" t="s">
+        <v>5</v>
+      </c>
+      <c r="C239" t="s">
+        <v>3</v>
+      </c>
+      <c r="D239" t="s">
+        <v>7</v>
+      </c>
+      <c r="E239" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A240" t="s">
+        <v>139</v>
+      </c>
+      <c r="B240" t="s">
+        <v>10</v>
+      </c>
+      <c r="C240" t="s">
+        <v>141</v>
+      </c>
+      <c r="D240" t="s">
+        <v>140</v>
+      </c>
+      <c r="E240" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="242" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A242" t="s">
+        <v>0</v>
+      </c>
+      <c r="B242" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A243" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A244" t="s">
+        <v>2</v>
+      </c>
+      <c r="B244" t="s">
+        <v>5</v>
+      </c>
+      <c r="C244" t="s">
+        <v>3</v>
+      </c>
+      <c r="D244" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="245" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A245" t="s">
+        <v>87</v>
+      </c>
+      <c r="B245" t="s">
+        <v>10</v>
+      </c>
+      <c r="C245" t="s">
+        <v>153</v>
+      </c>
+      <c r="D245" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="246" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A246" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="247" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A247" t="s">
+        <v>2</v>
+      </c>
+      <c r="B247" t="s">
+        <v>5</v>
+      </c>
+      <c r="C247" t="s">
+        <v>3</v>
+      </c>
+      <c r="D247" t="s">
+        <v>7</v>
+      </c>
+      <c r="E247" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="248" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A248" t="s">
+        <v>139</v>
+      </c>
+      <c r="B248" t="s">
+        <v>10</v>
+      </c>
+      <c r="C248" t="s">
+        <v>141</v>
+      </c>
+      <c r="D248" t="s">
+        <v>140</v>
+      </c>
+      <c r="E248" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="250" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A250" t="s">
+        <v>0</v>
+      </c>
+      <c r="B250" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="251" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A251" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="252" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A252" t="s">
+        <v>2</v>
+      </c>
+      <c r="B252" t="s">
+        <v>5</v>
+      </c>
+      <c r="C252" t="s">
+        <v>3</v>
+      </c>
+      <c r="D252" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="253" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A253" t="s">
+        <v>156</v>
+      </c>
+      <c r="B253" t="s">
+        <v>10</v>
+      </c>
+      <c r="C253" t="s">
+        <v>56</v>
+      </c>
+      <c r="D253" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="254" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A254" t="s">
+        <v>157</v>
+      </c>
+      <c r="B254" t="s">
+        <v>10</v>
+      </c>
+      <c r="C254" t="s">
+        <v>158</v>
+      </c>
+      <c r="D254" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="255" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A255" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="256" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A256" t="s">
+        <v>2</v>
+      </c>
+      <c r="B256" t="s">
+        <v>5</v>
+      </c>
+      <c r="C256" t="s">
+        <v>3</v>
+      </c>
+      <c r="D256" t="s">
+        <v>7</v>
+      </c>
+      <c r="E256" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="257" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A257" t="s">
+        <v>139</v>
+      </c>
+      <c r="B257" t="s">
+        <v>10</v>
+      </c>
+      <c r="C257" t="s">
+        <v>141</v>
+      </c>
+      <c r="D257" t="s">
+        <v>140</v>
+      </c>
+      <c r="E257" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="259" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A259" t="s">
+        <v>0</v>
+      </c>
+      <c r="B259" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="260" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A260" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="261" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A261" t="s">
+        <v>2</v>
+      </c>
+      <c r="B261" t="s">
+        <v>5</v>
+      </c>
+      <c r="C261" t="s">
+        <v>3</v>
+      </c>
+      <c r="D261" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="262" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A262" t="s">
+        <v>144</v>
+      </c>
+      <c r="B262" t="s">
+        <v>10</v>
+      </c>
+      <c r="C262" t="s">
+        <v>96</v>
+      </c>
+      <c r="D262" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="264" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A264" t="s">
+        <v>0</v>
+      </c>
+      <c r="B264" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="265" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A265" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="266" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A266" t="s">
+        <v>2</v>
+      </c>
+      <c r="B266" t="s">
+        <v>5</v>
+      </c>
+      <c r="C266" t="s">
+        <v>3</v>
+      </c>
+      <c r="D266" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="267" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A267" t="s">
+        <v>156</v>
+      </c>
+      <c r="B267" t="s">
+        <v>10</v>
+      </c>
+      <c r="C267" t="s">
+        <v>56</v>
+      </c>
+      <c r="D267" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="269" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A269" t="s">
+        <v>0</v>
+      </c>
+      <c r="B269" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="270" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A270" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="271" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A271" t="s">
+        <v>2</v>
+      </c>
+      <c r="B271" t="s">
+        <v>5</v>
+      </c>
+      <c r="C271" t="s">
+        <v>3</v>
+      </c>
+      <c r="D271" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="272" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A272" t="s">
+        <v>87</v>
+      </c>
+      <c r="B272" t="s">
+        <v>10</v>
+      </c>
+      <c r="C272" t="s">
+        <v>58</v>
+      </c>
+      <c r="D272" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="274" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A274" t="s">
+        <v>0</v>
+      </c>
+      <c r="B274" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="275" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A275" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="276" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A276" t="s">
+        <v>2</v>
+      </c>
+      <c r="B276" t="s">
+        <v>5</v>
+      </c>
+      <c r="C276" t="s">
+        <v>3</v>
+      </c>
+      <c r="D276" t="s">
+        <v>7</v>
+      </c>
+      <c r="E276" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="277" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A277" t="s">
+        <v>168</v>
+      </c>
+      <c r="B277" t="s">
+        <v>10</v>
+      </c>
+      <c r="C277" t="s">
+        <v>169</v>
+      </c>
+      <c r="D277" t="s">
+        <v>170</v>
+      </c>
+      <c r="E277" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="278" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A278" t="s">
+        <v>171</v>
+      </c>
+      <c r="B278" t="s">
+        <v>10</v>
+      </c>
+      <c r="C278" t="s">
+        <v>169</v>
+      </c>
+      <c r="D278" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E278" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="279" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A279" t="s">
+        <v>173</v>
+      </c>
+      <c r="B279" t="s">
+        <v>10</v>
+      </c>
+      <c r="C279" t="s">
+        <v>174</v>
+      </c>
+      <c r="D279" t="s">
+        <v>175</v>
+      </c>
+      <c r="E279" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="281" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A281" t="s">
+        <v>0</v>
+      </c>
+      <c r="B281" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="282" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A282" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="283" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A283" t="s">
+        <v>2</v>
+      </c>
+      <c r="B283" t="s">
+        <v>5</v>
+      </c>
+      <c r="C283" t="s">
+        <v>3</v>
+      </c>
+      <c r="D283" t="s">
+        <v>7</v>
+      </c>
+      <c r="E283" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="284" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A284" t="s">
+        <v>180</v>
+      </c>
+      <c r="B284" t="s">
+        <v>10</v>
+      </c>
+      <c r="C284" t="s">
+        <v>181</v>
+      </c>
+      <c r="D284" t="s">
+        <v>182</v>
+      </c>
+      <c r="E284" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="285" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D285" s="2"/>
+    </row>
+    <row r="286" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A286" t="s">
+        <v>0</v>
+      </c>
+      <c r="B286" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="287" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A287" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="288" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A288" t="s">
+        <v>2</v>
+      </c>
+      <c r="B288" t="s">
+        <v>5</v>
+      </c>
+      <c r="C288" t="s">
+        <v>3</v>
+      </c>
+      <c r="D288" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="289" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A289" t="s">
+        <v>185</v>
+      </c>
+      <c r="B289" t="s">
+        <v>10</v>
+      </c>
+      <c r="C289" t="s">
+        <v>141</v>
+      </c>
+      <c r="D289" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="290" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A290" t="s">
+        <v>189</v>
+      </c>
+      <c r="B290" t="s">
+        <v>10</v>
+      </c>
+      <c r="C290" t="s">
+        <v>190</v>
+      </c>
+      <c r="D290" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="291" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A291" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="292" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A292" t="s">
+        <v>2</v>
+      </c>
+      <c r="B292" t="s">
+        <v>5</v>
+      </c>
+      <c r="C292" t="s">
+        <v>3</v>
+      </c>
+      <c r="D292" t="s">
+        <v>7</v>
+      </c>
+      <c r="E292" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="293" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A293" t="s">
+        <v>180</v>
+      </c>
+      <c r="B293" t="s">
+        <v>10</v>
+      </c>
+      <c r="C293" t="s">
+        <v>181</v>
+      </c>
+      <c r="D293" t="s">
+        <v>111</v>
+      </c>
+      <c r="E293" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="294" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A294" t="s">
+        <v>187</v>
+      </c>
+      <c r="B294" t="s">
+        <v>10</v>
+      </c>
+      <c r="C294" t="s">
+        <v>141</v>
+      </c>
+      <c r="D294" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="E294" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="295" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A295" t="s">
+        <v>24</v>
+      </c>
+      <c r="B295" t="s">
+        <v>10</v>
+      </c>
+      <c r="C295" t="s">
+        <v>195</v>
+      </c>
+      <c r="D295" t="s">
+        <v>196</v>
+      </c>
+      <c r="E295" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="296" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A296" t="s">
+        <v>188</v>
+      </c>
+      <c r="B296" t="s">
+        <v>10</v>
+      </c>
+      <c r="C296" t="s">
+        <v>195</v>
+      </c>
+      <c r="D296" t="s">
+        <v>198</v>
+      </c>
+      <c r="E296" t="s">
+        <v>199</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Add PZ Refactoring Add Similarity Add circe for serialization Demonstration improvements
</commit_message>
<xml_diff>
--- a/Documentation/Class descriptions.xlsx
+++ b/Documentation/Class descriptions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pauldanilin/Documents/HSE/CourseWorks/HistogramModel/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CD3D197-BF38-D54A-A9C8-1944831F20AD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57719DDC-22DC-CC4F-A058-FC3DD4847614}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{0CA7BCAD-690E-1A42-B7BF-CE8354672EFF}"/>
   </bookViews>
@@ -991,7 +991,7 @@
   <dimension ref="A1:E296"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A275" zoomScale="150" workbookViewId="0">
-      <selection activeCell="E297" sqref="E297"/>
+      <selection activeCell="G284" sqref="G284"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>